<commit_message>
Update schließsysteme -> schließsysteme
</commit_message>
<xml_diff>
--- a/doc/wirtschaftsstruktur_parameter.xlsx
+++ b/doc/wirtschaftsstruktur_parameter.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PTT-MH\Documents\GitHub\PTT-API-Solutions\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839373D7-8457-494D-A2E0-1EF85341237B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26600" windowHeight="14900"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Wirtschaftsstruktur" sheetId="1" r:id="rId1"/>
@@ -12,17 +18,11 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -280,9 +280,6 @@
     <t>medien_und_marketing</t>
   </si>
   <si>
-    <t>schließsysteme_und_sicherheitstechnik</t>
-  </si>
-  <si>
     <t>tourismus_und_gastronomie</t>
   </si>
   <si>
@@ -347,13 +344,16 @@
   </si>
   <si>
     <t>alterative request parameter</t>
+  </si>
+  <si>
+    <t>schliesssysteme_und_sicherheitstechnik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,46 +823,46 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="15">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1">
       <c r="A3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -983,7 +983,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1016,7 +1016,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1104,7 +1104,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1115,7 +1115,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1159,7 +1159,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1170,7 +1170,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1181,7 +1181,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1203,7 +1203,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1214,7 +1214,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1225,7 +1225,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1236,7 +1236,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1269,7 +1269,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1291,7 +1291,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1313,7 +1313,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1379,7 +1379,7 @@
         <v>46</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1390,7 +1390,7 @@
         <v>47</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1423,7 +1423,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1442,16 +1442,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>